<commit_message>
genus 100% 로, click & mouse over
</commit_message>
<xml_diff>
--- a/crs_table_filtered_genus.xlsx
+++ b/crs_table_filtered_genus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="26680" windowHeight="12880" tabRatio="500"/>
+    <workbookView xWindow="13660" yWindow="460" windowWidth="13660" windowHeight="13660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -16019,11 +16019,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1354132240"/>
-        <c:axId val="-1324333680"/>
+        <c:axId val="-1047428016"/>
+        <c:axId val="-1047426656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1354132240"/>
+        <c:axId val="-1047428016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16033,7 +16033,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1324333680"/>
+        <c:crossAx val="-1047426656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16041,7 +16041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1324333680"/>
+        <c:axId val="-1047426656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16051,7 +16051,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1354132240"/>
+        <c:crossAx val="-1047428016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16373,8 +16373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>